<commit_message>
Pridana schema s OZ a bez OZ pre varianty
</commit_message>
<xml_diff>
--- a/Production/M74R2_Pasiv_bez_OZ_BOM.xlsx
+++ b/Production/M74R2_Pasiv_bez_OZ_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\M74R\Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D07A5A-37EB-4D14-86C2-8AF36049FC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42377459-753B-46D8-AD46-A62E98EBDC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42555" yWindow="2385" windowWidth="26955" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="280" windowWidth="21010" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M74R2_Pasiv_bez_OZ_BOM" sheetId="1" r:id="rId1"/>
@@ -989,16 +989,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7265625" customWidth="1"/>
     <col min="3" max="3" width="19.90625" customWidth="1"/>
     <col min="4" max="6" width="16.7265625" customWidth="1"/>
@@ -1103,7 +1102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>0</v>
       </c>
@@ -1318,7 +1317,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>0</v>
       </c>
@@ -1402,7 +1401,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>0</v>
       </c>
@@ -1443,7 +1442,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>0</v>
       </c>
@@ -1525,7 +1524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>0</v>
       </c>
@@ -1644,7 +1643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>0</v>
       </c>
@@ -1685,7 +1684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>0</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>0</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>0</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>0</v>
       </c>
@@ -2056,7 +2055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>0</v>
       </c>
@@ -2097,7 +2096,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>0</v>
       </c>
@@ -2138,7 +2137,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>0</v>
       </c>
@@ -2220,7 +2219,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>0</v>
       </c>
@@ -2261,7 +2260,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>0</v>
       </c>
@@ -2300,7 +2299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>0</v>
       </c>
@@ -2457,13 +2456,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O35" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="14">
-      <filters>
-        <filter val="Fitted"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>